<commit_message>
updated api end points of L1 ,L2  and  DM
</commit_message>
<xml_diff>
--- a/L1_candidates.xlsx
+++ b/L1_candidates.xlsx
@@ -367,13 +367,13 @@
     </row>
     <row r="3">
       <c r="B3">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="C3" t="str">
-        <v>tishya</v>
+        <v>naman roy</v>
       </c>
       <c r="D3" t="str">
-        <v>tishya@gmail.com</v>
+        <v>roy1998@gmail.com</v>
       </c>
       <c r="E3" t="str">
         <v>globalTiger</v>
@@ -382,7 +382,7 @@
         <v>55667788</v>
       </c>
       <c r="G3" t="str">
-        <v>L1_rejected</v>
+        <v>L1_selected</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating in pending status(TBS OR scheduled) for L1,L2,DM
</commit_message>
<xml_diff>
--- a/L1_candidates.xlsx
+++ b/L1_candidates.xlsx
@@ -367,13 +367,13 @@
     </row>
     <row r="3">
       <c r="B3">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C3" t="str">
-        <v>naman roy</v>
+        <v>tishya</v>
       </c>
       <c r="D3" t="str">
-        <v>roy1998@gmail.com</v>
+        <v>tishya@gmail.com</v>
       </c>
       <c r="E3" t="str">
         <v>globalTiger</v>
@@ -382,7 +382,67 @@
         <v>55667788</v>
       </c>
       <c r="G3" t="str">
+        <v>L1_rejected</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4">
+        <v>314</v>
+      </c>
+      <c r="C4" t="str">
+        <v>naman roy</v>
+      </c>
+      <c r="D4" t="str">
+        <v>roy1998@gmail.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>globalTiger</v>
+      </c>
+      <c r="F4" t="str">
+        <v>55667788</v>
+      </c>
+      <c r="G4" t="str">
         <v>L1_selected</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5">
+        <v>315</v>
+      </c>
+      <c r="C5" t="str">
+        <v>peter griffin</v>
+      </c>
+      <c r="D5" t="str">
+        <v>peter@gmail.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>nasa</v>
+      </c>
+      <c r="F5" t="str">
+        <v>55667799</v>
+      </c>
+      <c r="G5" t="str">
+        <v>L1_TBS</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6">
+        <v>316</v>
+      </c>
+      <c r="C6" t="str">
+        <v>surma</v>
+      </c>
+      <c r="D6" t="str">
+        <v>surma@gmail.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>umbrala corporation</v>
+      </c>
+      <c r="F6" t="str">
+        <v>55667788</v>
+      </c>
+      <c r="G6" t="str">
+        <v>L1_scheduled</v>
       </c>
     </row>
   </sheetData>

</xml_diff>